<commit_message>
Add stress test report
</commit_message>
<xml_diff>
--- a/booking-api-test-report.xlsx
+++ b/booking-api-test-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumai\Downloads\Assignment\Assignment 3 Jmeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA08CF79-03C2-44C2-B11F-E602E333EAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF9283C-0E60-4942-95FB-967DD8C26010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
   <si>
     <t>Step</t>
   </si>
@@ -97,13 +97,43 @@
   </si>
   <si>
     <t>2.75</t>
+  </si>
+  <si>
+    <t>0.10%</t>
+  </si>
+  <si>
+    <t>0.12%</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>2.83</t>
+  </si>
+  <si>
+    <t>0.15%</t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t>0.17%</t>
+  </si>
+  <si>
+    <t>Assuming company accepts error rate less than or equal to 0.15</t>
+  </si>
+  <si>
+    <t>2.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.95  Bottleneck throughput </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +164,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3D3D3D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,7 +216,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +224,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -577,16 +615,16 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>5</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>300</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>833</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -594,10 +632,10 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="H5" s="6" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="H5" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -605,10 +643,10 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="H6" s="6" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -616,10 +654,10 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>10</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="2"/>
@@ -631,14 +669,14 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
         <v>600</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1666</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -646,9 +684,9 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
       <c r="H9" s="2" t="s">
         <v>23</v>
       </c>
@@ -657,9 +695,9 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="H10" s="2" t="s">
         <v>24</v>
       </c>
@@ -668,7 +706,7 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="2"/>
@@ -680,13 +718,13 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>20</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>1200</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>3333</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -697,9 +735,9 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="H13" s="2" t="s">
         <v>23</v>
       </c>
@@ -708,9 +746,9 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="H14" s="2">
         <v>2.76</v>
       </c>
@@ -742,10 +780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482C672A-B60A-48F6-9687-F42136622F27}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D6"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,6 +793,7 @@
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -824,40 +863,45 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8">
-        <v>6</v>
-      </c>
-      <c r="E4" s="8">
-        <v>660</v>
-      </c>
-      <c r="F4" s="8">
-        <v>833</v>
+      <c r="D4" s="7">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7">
+        <v>600</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1666</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>10</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -866,36 +910,39 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
         <v>600</v>
       </c>
-      <c r="F8" s="8">
-        <v>1666</v>
+      <c r="F8" s="7">
+        <v>1676</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>18</v>
+      <c r="G11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -905,42 +952,189 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8">
-        <v>20</v>
-      </c>
-      <c r="E12" s="8">
-        <v>1200</v>
-      </c>
-      <c r="F12" s="8">
-        <v>3333</v>
+      <c r="D12" s="7">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7">
+        <v>600</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1700</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>16</v>
+      <c r="G15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="7">
+        <v>10</v>
+      </c>
+      <c r="E16" s="7">
+        <v>600</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="7">
+        <v>10</v>
+      </c>
+      <c r="E20" s="7">
+        <v>600</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="7">
+        <v>10</v>
+      </c>
+      <c r="E24" s="7">
+        <v>600</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>

</xml_diff>